<commit_message>
Rescus .rels files, re-process
</commit_message>
<xml_diff>
--- a/inst/extdata/types.xlsx
+++ b/inst/extdata/types.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26915"/>
-  <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26915"/>
+  <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jenny/rrr/readxl/tests/testthat/sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6720" yWindow="920" windowWidth="20980" windowHeight="13980" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="2880" yWindow="1160" windowWidth="20980" windowHeight="13980" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="guess_me" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="44">
   <si>
     <t>ab</t>
   </si>
@@ -126,6 +126,45 @@
   </si>
   <si>
     <t>foo</t>
+  </si>
+  <si>
+    <t>72</t>
+  </si>
+  <si>
+    <t>explanation</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>False</t>
+  </si>
+  <si>
+    <t>static logical</t>
+  </si>
+  <si>
+    <t>formula logical</t>
+  </si>
+  <si>
+    <t>string logical</t>
+  </si>
+  <si>
+    <t>string not logical</t>
+  </si>
+  <si>
+    <t>logical F</t>
+  </si>
+  <si>
+    <t>floating point</t>
   </si>
 </sst>
 </file>
@@ -153,9 +192,18 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -165,10 +213,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -506,7 +559,7 @@
   <dimension ref="B1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -609,7 +662,7 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E1048576"/>
+      <selection sqref="A1:E65536"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -827,10 +880,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B8"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -838,45 +891,149 @@
     <col min="1" max="2" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A3" t="str">
-        <f>"F"</f>
-        <v>F</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A4" t="s">
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3" t="b">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A4" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A5" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A6" t="str">
+        <f>"true"</f>
+        <v>true</v>
+      </c>
+      <c r="B6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A7" t="str">
+        <f>"false"</f>
+        <v>false</v>
+      </c>
+      <c r="B7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A8" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A9" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A12" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A13" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A14" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A5">
+      <c r="B14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A16">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A7" s="1">
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A18" s="1">
         <v>40908</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A8" t="b">
-        <v>0</v>
+      <c r="B18" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -893,6 +1050,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
@@ -920,8 +1080,8 @@
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A7" s="1">
-        <v>39529</v>
+      <c r="A7" s="4">
+        <v>39448</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.15">
@@ -939,7 +1099,7 @@
   <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -958,8 +1118,8 @@
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A3">
-        <v>-2</v>
+      <c r="A3" s="3" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.15">
@@ -989,10 +1149,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1000,39 +1160,65 @@
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>1.3</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" s="1">
         <v>41175</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>30</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>